<commit_message>
Added other text to Hardware, written the first version of Abstract, added Bibliography and Index.
</commit_message>
<xml_diff>
--- a/thesis/RequirementsHW.xlsx
+++ b/thesis/RequirementsHW.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Requirements" sheetId="1" r:id="rId1"/>
+    <sheet name="Errata" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="60">
   <si>
     <t>Category</t>
   </si>
@@ -117,6 +118,93 @@
   </si>
   <si>
     <t>Outdoor use</t>
+  </si>
+  <si>
+    <t>Number</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Image</t>
+  </si>
+  <si>
+    <t>Severity</t>
+  </si>
+  <si>
+    <t>Panelization bridge under micro USB connector</t>
+  </si>
+  <si>
+    <t>Error created during</t>
+  </si>
+  <si>
+    <t>panelization</t>
+  </si>
+  <si>
+    <t>schematics design</t>
+  </si>
+  <si>
+    <t>Swapped MISO and MOSI on pins IO19 and IO21 on the ESP-WROOM-32 chip according to ESP32 Arduino standard</t>
+  </si>
+  <si>
+    <t>Severity:</t>
+  </si>
+  <si>
+    <t>The prototype has to be remade</t>
+  </si>
+  <si>
+    <t>Some part of the prototype may not work</t>
+  </si>
+  <si>
+    <t>No significant affects</t>
+  </si>
+  <si>
+    <t>What happens</t>
+  </si>
+  <si>
+    <t>The micro USB connector may be placed with lower accuracy</t>
+  </si>
+  <si>
+    <t>The SPI interface is not working in Arduino compatible mode without modification of the Arduino SPI library</t>
+  </si>
+  <si>
+    <t>LED5 connected to IO35 on ESP-WROOM-32 is not working</t>
+  </si>
+  <si>
+    <t>The pins IO34 -- IO39 are input only, so they cannot drive a LED</t>
+  </si>
+  <si>
+    <t>Spare</t>
+  </si>
+  <si>
+    <t>Only spare devices may not work</t>
+  </si>
+  <si>
+    <t>Missing pull-up resistors on SD card</t>
+  </si>
+  <si>
+    <t>The SDIO interface needs external pull-up resistors to work properly. I have added these resistors later by hand.</t>
+  </si>
+  <si>
+    <t>The temperature measurement is placed very close to the main processor</t>
+  </si>
+  <si>
+    <t>board layout</t>
+  </si>
+  <si>
+    <t>The processor heating affects the measured temperature</t>
+  </si>
+  <si>
+    <t>Low capacity capacitor plased on power supply</t>
+  </si>
+  <si>
+    <t>When we use WiFi some brownouts can be detected. I have added a bigger capacitor later by hand.</t>
+  </si>
+  <si>
+    <t>The light sensor is placed on inner side of the board</t>
+  </si>
+  <si>
+    <t>The measured values are affected by shadow of the board</t>
   </si>
 </sst>
 </file>
@@ -470,7 +558,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+    <sheetView topLeftCell="A17" workbookViewId="0">
       <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
@@ -639,4 +727,201 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="25.42578125" customWidth="1"/>
+    <col min="3" max="3" width="22.28515625" customWidth="1"/>
+    <col min="4" max="4" width="16.85546875" customWidth="1"/>
+    <col min="5" max="5" width="11.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D10" t="s">
+        <v>44</v>
+      </c>
+      <c r="E10" t="s">
+        <v>33</v>
+      </c>
+      <c r="F10" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>1</v>
+      </c>
+      <c r="B11" t="s">
+        <v>35</v>
+      </c>
+      <c r="C11" t="s">
+        <v>37</v>
+      </c>
+      <c r="D11" t="s">
+        <v>45</v>
+      </c>
+      <c r="F11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>2</v>
+      </c>
+      <c r="B12" t="s">
+        <v>39</v>
+      </c>
+      <c r="C12" t="s">
+        <v>38</v>
+      </c>
+      <c r="D12" t="s">
+        <v>46</v>
+      </c>
+      <c r="F12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>3</v>
+      </c>
+      <c r="B13" t="s">
+        <v>47</v>
+      </c>
+      <c r="C13" t="s">
+        <v>38</v>
+      </c>
+      <c r="D13" t="s">
+        <v>48</v>
+      </c>
+      <c r="F13" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>4</v>
+      </c>
+      <c r="B14" t="s">
+        <v>51</v>
+      </c>
+      <c r="C14" t="s">
+        <v>38</v>
+      </c>
+      <c r="D14" t="s">
+        <v>52</v>
+      </c>
+      <c r="F14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>5</v>
+      </c>
+      <c r="B15" t="s">
+        <v>53</v>
+      </c>
+      <c r="C15" t="s">
+        <v>54</v>
+      </c>
+      <c r="D15" t="s">
+        <v>55</v>
+      </c>
+      <c r="F15" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>6</v>
+      </c>
+      <c r="B16" t="s">
+        <v>56</v>
+      </c>
+      <c r="C16" t="s">
+        <v>38</v>
+      </c>
+      <c r="D16" t="s">
+        <v>57</v>
+      </c>
+      <c r="F16" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>7</v>
+      </c>
+      <c r="B17" t="s">
+        <v>58</v>
+      </c>
+      <c r="C17" t="s">
+        <v>54</v>
+      </c>
+      <c r="D17" t="s">
+        <v>59</v>
+      </c>
+      <c r="F17" t="s">
+        <v>49</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>